<commit_message>
QUAD MAX ENT RESULTS ARE GOOD!!!!!!
</commit_message>
<xml_diff>
--- a/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
+++ b/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhackemack\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\outputs\Transport_MMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\outputs\Transport_MMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -901,11 +901,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199999360"/>
-        <c:axId val="199997120"/>
+        <c:axId val="233500424"/>
+        <c:axId val="233501600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199999360"/>
+        <c:axId val="233500424"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -965,12 +965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199997120"/>
+        <c:crossAx val="233501600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199997120"/>
+        <c:axId val="233501600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1028,7 +1028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199999360"/>
+        <c:crossAx val="233500424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1493,7 +1493,19 @@
                   <c:v>2088</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5192</c:v>
+                  <c:v>5264</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33970</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83566</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>207442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1529,19 @@
                   <c:v>1.5775708986585199E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3882643757812002E-4</c:v>
+                  <c:v>3.9143596309961301E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1535960015255E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2.8819047517352001E-5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>6.9004676165009799E-6</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>2.1959838350590502E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1656,11 +1680,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="34425312"/>
-        <c:axId val="34424752"/>
+        <c:axId val="233497680"/>
+        <c:axId val="233505128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34425312"/>
+        <c:axId val="233497680"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1682,6 +1706,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># DoFs</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1719,12 +1799,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34424752"/>
+        <c:crossAx val="233505128"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="34424752"/>
+        <c:axId val="233505128"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1745,6 +1825,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>||u-uh||</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1782,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34425312"/>
+        <c:crossAx val="233497680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2386,11 +2522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="328441408"/>
-        <c:axId val="328441968"/>
+        <c:axId val="203976296"/>
+        <c:axId val="203973944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="328441408"/>
+        <c:axId val="203976296"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2448,12 +2584,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328441968"/>
+        <c:crossAx val="203973944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="328441968"/>
+        <c:axId val="203973944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2511,7 +2647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328441408"/>
+        <c:crossAx val="203976296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2981,11 +3117,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="328446448"/>
-        <c:axId val="328447008"/>
+        <c:axId val="203975120"/>
+        <c:axId val="203972376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="328446448"/>
+        <c:axId val="203975120"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3043,12 +3179,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328447008"/>
+        <c:crossAx val="203972376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="328447008"/>
+        <c:axId val="203972376"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3106,7 +3242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328446448"/>
+        <c:crossAx val="203975120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3493,11 +3629,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="328937616"/>
-        <c:axId val="328938176"/>
+        <c:axId val="203970808"/>
+        <c:axId val="317563896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="328937616"/>
+        <c:axId val="203970808"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3555,12 +3691,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328938176"/>
+        <c:crossAx val="317563896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="328938176"/>
+        <c:axId val="317563896"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3618,7 +3754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328937616"/>
+        <c:crossAx val="203970808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7236,7 +7372,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7668,10 +7804,10 @@
         <v>5.8092842763180601E-3</v>
       </c>
       <c r="Q7">
-        <v>5192</v>
+        <v>5264</v>
       </c>
       <c r="R7">
-        <v>4.3882643757812002E-4</v>
+        <v>3.9143596309961301E-4</v>
       </c>
       <c r="S7">
         <v>2244</v>
@@ -7734,6 +7870,12 @@
       <c r="P8" s="13">
         <v>8.0587555871336602E-3</v>
       </c>
+      <c r="Q8">
+        <v>13444</v>
+      </c>
+      <c r="R8">
+        <v>1.1535960015255E-4</v>
+      </c>
       <c r="S8">
         <v>4240</v>
       </c>
@@ -7779,6 +7921,12 @@
       <c r="P9" s="13">
         <v>1.3073030878355599E-2</v>
       </c>
+      <c r="Q9">
+        <v>33970</v>
+      </c>
+      <c r="R9" s="16">
+        <v>2.8819047517352001E-5</v>
+      </c>
       <c r="S9">
         <v>8252</v>
       </c>
@@ -7793,6 +7941,12 @@
       <c r="P10" s="13">
         <v>2.15593843417007E-2</v>
       </c>
+      <c r="Q10">
+        <v>83566</v>
+      </c>
+      <c r="R10" s="16">
+        <v>6.9004676165009799E-6</v>
+      </c>
       <c r="S10">
         <v>15360</v>
       </c>
@@ -7806,6 +7960,12 @@
       </c>
       <c r="P11" s="13">
         <v>6.1220770443589203E-3</v>
+      </c>
+      <c r="Q11">
+        <v>207442</v>
+      </c>
+      <c r="R11" s="16">
+        <v>2.1959838350590502E-6</v>
       </c>
       <c r="S11">
         <v>29736</v>

</xml_diff>

<commit_message>
vtk output for k>1 in 2D
</commit_message>
<xml_diff>
--- a/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
+++ b/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
@@ -901,11 +901,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233500424"/>
-        <c:axId val="233501600"/>
+        <c:axId val="200222512"/>
+        <c:axId val="200223296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233500424"/>
+        <c:axId val="200222512"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -965,12 +965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233501600"/>
+        <c:crossAx val="200223296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233501600"/>
+        <c:axId val="200223296"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1028,7 +1028,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233500424"/>
+        <c:crossAx val="200222512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1680,11 +1680,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="233497680"/>
-        <c:axId val="233505128"/>
+        <c:axId val="200224080"/>
+        <c:axId val="200224472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="233497680"/>
+        <c:axId val="200224080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1799,12 +1799,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233505128"/>
+        <c:crossAx val="200224472"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="233505128"/>
+        <c:axId val="200224472"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1918,7 +1918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="233497680"/>
+        <c:crossAx val="200224080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2522,11 +2522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203976296"/>
-        <c:axId val="203973944"/>
+        <c:axId val="200225256"/>
+        <c:axId val="200225648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203976296"/>
+        <c:axId val="200225256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2584,12 +2584,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203973944"/>
+        <c:crossAx val="200225648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203973944"/>
+        <c:axId val="200225648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2647,7 +2647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203976296"/>
+        <c:crossAx val="200225256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3117,11 +3117,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203975120"/>
-        <c:axId val="203972376"/>
+        <c:axId val="200226432"/>
+        <c:axId val="200226824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203975120"/>
+        <c:axId val="200226432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3179,12 +3179,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203972376"/>
+        <c:crossAx val="200226824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203972376"/>
+        <c:axId val="200226824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3242,7 +3242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203975120"/>
+        <c:crossAx val="200226432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3629,11 +3629,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203970808"/>
-        <c:axId val="317563896"/>
+        <c:axId val="200227608"/>
+        <c:axId val="200228000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203970808"/>
+        <c:axId val="200227608"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3691,12 +3691,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317563896"/>
+        <c:crossAx val="200228000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="317563896"/>
+        <c:axId val="200228000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3754,7 +3754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203970808"/>
+        <c:crossAx val="200227608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6654,15 +6654,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>549085</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>56028</xdr:rowOff>
+      <xdr:colOff>156878</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>728381</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>750793</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7372,7 +7372,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected mms limit functions
</commit_message>
<xml_diff>
--- a/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
+++ b/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\outputs\Transport_MMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhackemack\Documents\GitHub\POLYFEM2\Codes\MATLAB\POLYFEM\outputs\Transport_MMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="737" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Gauss_2D_quads_iso DFEM Linear" sheetId="1" r:id="rId1"/>
-    <sheet name="Gauss_2D_quads_iso - Quadratic" sheetId="2" r:id="rId2"/>
-    <sheet name="G2D_quads_Lagrange" sheetId="6" r:id="rId3"/>
-    <sheet name="Gauss_2D_quads_iso CFEM lin" sheetId="3" r:id="rId4"/>
-    <sheet name="QuadSol_1angle - DFEM lin" sheetId="4" r:id="rId5"/>
-    <sheet name="QuadSol_1angle - DFEM quad" sheetId="5" r:id="rId6"/>
+    <sheet name="Gauss_2D_iso - Quadratic" sheetId="2" r:id="rId2"/>
+    <sheet name="Quad_2D_iso" sheetId="7" r:id="rId3"/>
+    <sheet name="G2D_quads_Lagrange" sheetId="6" r:id="rId4"/>
+    <sheet name="Gauss_2D_quads_iso CFEM lin" sheetId="3" r:id="rId5"/>
+    <sheet name="QuadSol_1angle - DFEM lin" sheetId="4" r:id="rId6"/>
+    <sheet name="QuadSol_1angle - DFEM quad" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="45">
   <si>
     <t>Uniform</t>
   </si>
@@ -129,6 +130,42 @@
   <si>
     <t>Random Poly Mesh</t>
   </si>
+  <si>
+    <t>PWLD</t>
+  </si>
+  <si>
+    <t>MAXENT</t>
+  </si>
+  <si>
+    <t>Polygonal</t>
+  </si>
+  <si>
+    <t>Smooth</t>
+  </si>
+  <si>
+    <t>Z-Mesh</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>Quadratic</t>
+  </si>
+  <si>
+    <t>Dofs</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Shestakov</t>
+  </si>
 </sst>
 </file>
 
@@ -151,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -239,11 +276,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,6 +436,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -347,6 +467,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,11 +1084,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214601584"/>
-        <c:axId val="214601968"/>
+        <c:axId val="151397280"/>
+        <c:axId val="151397840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214601584"/>
+        <c:axId val="151397280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -986,12 +1148,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214601968"/>
+        <c:crossAx val="151397840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214601968"/>
+        <c:axId val="151397840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1049,7 +1211,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214601584"/>
+        <c:crossAx val="151397280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1138,7 +1300,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$A$3:$A$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1168,7 +1330,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$G$3:$G$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1219,7 +1381,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$A$3:$A$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1249,7 +1411,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$H$3:$H$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1311,7 +1473,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$A$3:$A$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$A$3:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1341,7 +1503,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$E$3:$E$9</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1403,7 +1565,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$M$3:$M$8</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$M$3:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1430,7 +1592,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$N$3:$N$8</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$N$3:$N$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1462,7 +1624,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$Q$1:$R$1</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$Q$1:$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1497,7 +1659,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$Q$3:$Q$15</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$Q$3:$Q$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1533,7 +1695,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$R$3:$R$15</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$R$3:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1574,7 +1736,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$S$1:$T$1</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$S$1:$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1609,7 +1771,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$S$3:$S$15</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$S$3:$S$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1651,7 +1813,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$T$3:$T$15</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$T$3:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1731,7 +1893,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$U$3:$U$13</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$U$3:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1755,7 +1917,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$V$3:$V$13</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$V$3:$V$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1817,7 +1979,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$W$3:$W$13</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$W$3:$W$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1844,7 +2006,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Gauss_2D_quads_iso - Quadratic'!$X$3:$X$13</c:f>
+              <c:f>'Gauss_2D_iso - Quadratic'!$X$3:$X$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1879,11 +2041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214907944"/>
-        <c:axId val="214908328"/>
+        <c:axId val="198394272"/>
+        <c:axId val="198394832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214907944"/>
+        <c:axId val="198394272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1998,12 +2160,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214908328"/>
+        <c:crossAx val="198394832"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214908328"/>
+        <c:axId val="198394832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2117,7 +2279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214907944"/>
+        <c:crossAx val="198394272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2212,6 +2374,685 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1440" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Quad_2D_iso!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>First</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$C$2:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.90625E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.765625E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.44140625E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.103515625E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5999999999999999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Quad_2D_iso!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Second</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$D$2:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>7.8125E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.765625E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.220703125E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.52587890625E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9073486328125E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.384185791015625E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2000000000000001E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Uniform - Linear MAXENT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$E$5:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65536</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$F$5:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.82072280697912903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.206660698989033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1812164029267901E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2968167697866699E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2436799318507899E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1110695211347597E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Uniform - Quadratic MAXENT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$O$5:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$P$5:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>5.6910399790446098E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2707237794323301E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2094511558979701E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.16770295444356E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>1.51326488849241E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>2.1250912616835202E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$Q$5:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Quad_2D_iso!$R$5:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.20549063061801801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0742880682756202E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.44469986169836E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9808011726754099E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2034561665896399E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="264576304"/>
+        <c:axId val="264575744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="264576304"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264575744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="264575744"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="264576304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
@@ -2721,11 +3562,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215174760"/>
-        <c:axId val="214446744"/>
+        <c:axId val="198400432"/>
+        <c:axId val="198400992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215174760"/>
+        <c:axId val="198400432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2783,12 +3624,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214446744"/>
+        <c:crossAx val="198400992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214446744"/>
+        <c:axId val="198400992"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2846,602 +3687,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215174760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$A$4:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65536</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$B$4:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.4633255085630798E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1034296750803901E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7422973251359098E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8360800833021796E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7067869013473301E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>4.2645913129575001E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$A$4:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65536</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$C$4:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.4817675982742E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.10920064465893E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7582070447413299E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.8777383499310995E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7174388682753201E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>4.2915181519391997E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$E$4:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1536</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6144</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24576</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>98304</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$G$4:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.8081826404001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1925167890795001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9663920547648602E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.3970942806215003E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8471442224791301E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>4.6157088931970002E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$E$4:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>384</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1536</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6144</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24576</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>98304</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM lin'!$H$4:$H$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4.8081826404148702E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1925167891111499E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9663920550908598E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.3970942839033901E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.84714422579695E-4</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>4.61570892665915E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="214562944"/>
-        <c:axId val="214563328"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="214562944"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="214563328"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="214563328"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="214562944"/>
+        <c:crossAx val="198400432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3600,54 +3846,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$A$4:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>768</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3072</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12288</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49152</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>196608</c:v>
+                  <c:v>65536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$D$4:$D$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.4999015316313201E-2</c:v>
+                  <c:v>4.4633255085630798E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7670900456358201E-3</c:v>
+                  <c:v>1.1034296750803901E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4470058220417498E-4</c:v>
+                  <c:v>2.7422973251359098E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3662422981680101E-4</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>5.9222760256350099E-5</c:v>
+                  <c:v>6.8360800833021796E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7067869013473301E-4</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00E+00">
-                  <c:v>1.4815466809758699E-5</c:v>
+                  <c:v>4.2645913129575001E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3683,54 +3929,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$A$4:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>768</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3072</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12288</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49152</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>196608</c:v>
+                  <c:v>65536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$E$4:$E$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.208333333333333E-3</c:v>
+                  <c:v>4.4817675982742E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3020833333333333E-3</c:v>
+                  <c:v>1.10920064465893E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2552083333333332E-4</c:v>
+                  <c:v>2.7582070447413299E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1380208333333329E-5</c:v>
+                  <c:v>6.8777383499310995E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0345052083333332E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.0862630208333331E-6</c:v>
+                  <c:v>1.7174388682753201E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>4.2915181519391997E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3766,54 +4012,137 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>192</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>768</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3072</c:v>
+                  <c:v>1536</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12288</c:v>
+                  <c:v>6144</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49152</c:v>
+                  <c:v>24576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>196608</c:v>
+                  <c:v>98304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'QuadSol_1angle - DFEM quad'!$F$4:$F$9</c:f>
+              <c:f>'QuadSol_1angle - DFEM lin'!$G$4:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.7587908150366268E-4</c:v>
+                  <c:v>4.8081826404001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6984885187957773E-5</c:v>
+                  <c:v>1.1925167890795001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.873110648494731E-6</c:v>
+                  <c:v>2.9663920547648602E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3413883106183989E-7</c:v>
+                  <c:v>7.3970942806215003E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1767353882730132E-8</c:v>
+                  <c:v>1.8471442224791301E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>4.6157088931970002E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM lin'!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24576</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1470919235341242E-8</c:v>
+                  <c:v>98304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM lin'!$H$4:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.8081826404148702E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1925167891111499E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9663920550908598E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3970942839033901E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.84714422579695E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>4.61570892665915E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3828,11 +4157,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215058640"/>
-        <c:axId val="215059024"/>
+        <c:axId val="198405472"/>
+        <c:axId val="198406032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215058640"/>
+        <c:axId val="198405472"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3890,12 +4219,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215059024"/>
+        <c:crossAx val="198406032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215059024"/>
+        <c:axId val="198406032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3953,7 +4282,519 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215058640"/>
+        <c:crossAx val="198405472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$D$4:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4999015316313201E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7670900456358201E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4470058220417498E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3662422981680101E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>5.9222760256350099E-5</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00E+00">
+                  <c:v>1.4815466809758699E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$E$4:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.208333333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3020833333333333E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2552083333333332E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1380208333333329E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0345052083333332E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0862630208333331E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$C$4:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3072</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49152</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196608</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'QuadSol_1angle - DFEM quad'!$F$4:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.7587908150366268E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6984885187957773E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.873110648494731E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3413883106183989E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1767353882730132E-8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1470919235341242E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="199195968"/>
+        <c:axId val="199196528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="199195968"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="199196528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="199196528"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="199195968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4233,6 +5074,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6298,6 +7179,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6887,6 +8284,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>312963</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>50346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>707571</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -6918,7 +8350,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6953,7 +8385,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7267,17 +8699,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -7570,8 +9002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7595,51 +9027,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="J1" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25" t="s">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="26" t="s">
+      <c r="T1" s="26"/>
+      <c r="U1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="26"/>
-      <c r="W1" s="25" t="s">
+      <c r="V1" s="27"/>
+      <c r="W1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25" t="s">
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="26" t="s">
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="26"/>
+      <c r="AB1" s="27"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -8411,6 +9843,812 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11.7109375" style="25" customWidth="1"/>
+    <col min="5" max="23" width="13.7109375" style="25" customWidth="1"/>
+    <col min="24" max="31" width="9.140625" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
+        <v>64</v>
+      </c>
+      <c r="B2" s="25">
+        <f>0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="C2" s="25">
+        <f>B2^2*10</f>
+        <v>0.625</v>
+      </c>
+      <c r="D2" s="25">
+        <f>B2^3*5</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="42"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>256</v>
+      </c>
+      <c r="B3" s="25">
+        <f>B2/2</f>
+        <v>0.125</v>
+      </c>
+      <c r="C3" s="25">
+        <f t="shared" ref="C3:C8" si="0">B3^2*10</f>
+        <v>0.15625</v>
+      </c>
+      <c r="D3" s="25">
+        <f t="shared" ref="D3:D8" si="1">B3^3*5</f>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="42"/>
+      <c r="M3" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="42"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>1024</v>
+      </c>
+      <c r="B4" s="25">
+        <f t="shared" ref="B4:B7" si="2">B3/2</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C4" s="25">
+        <f t="shared" si="0"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="D4" s="25">
+        <f t="shared" si="1"/>
+        <v>1.220703125E-3</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" s="45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>4096</v>
+      </c>
+      <c r="B5" s="25">
+        <f t="shared" si="2"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="C5" s="25">
+        <f t="shared" si="0"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="D5" s="25">
+        <f t="shared" si="1"/>
+        <v>1.52587890625E-4</v>
+      </c>
+      <c r="E5" s="43">
+        <v>64</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0.82072280697912903</v>
+      </c>
+      <c r="G5" s="44">
+        <v>64</v>
+      </c>
+      <c r="H5" s="44">
+        <v>0.75988362489888905</v>
+      </c>
+      <c r="I5" s="44">
+        <v>36</v>
+      </c>
+      <c r="J5" s="44">
+        <v>2.2850999999999999</v>
+      </c>
+      <c r="K5" s="44">
+        <v>80</v>
+      </c>
+      <c r="L5" s="46">
+        <v>13.6046176508166</v>
+      </c>
+      <c r="M5" s="43">
+        <v>144</v>
+      </c>
+      <c r="N5" s="47">
+        <v>6.4219373632584602E-15</v>
+      </c>
+      <c r="O5" s="47">
+        <v>128</v>
+      </c>
+      <c r="P5" s="47">
+        <v>5.6910399790446098E-2</v>
+      </c>
+      <c r="Q5" s="44">
+        <v>72</v>
+      </c>
+      <c r="R5" s="47">
+        <v>0.20549063061801801</v>
+      </c>
+      <c r="S5" s="44">
+        <v>160</v>
+      </c>
+      <c r="T5" s="47">
+        <v>0.15065920556939599</v>
+      </c>
+      <c r="U5" s="44">
+        <v>88</v>
+      </c>
+      <c r="V5" s="46">
+        <v>0.34221106093520298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>16384</v>
+      </c>
+      <c r="B6" s="25">
+        <f t="shared" si="2"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="C6" s="25">
+        <f t="shared" si="0"/>
+        <v>2.44140625E-3</v>
+      </c>
+      <c r="D6" s="25">
+        <f t="shared" si="1"/>
+        <v>1.9073486328125E-5</v>
+      </c>
+      <c r="E6" s="43">
+        <v>256</v>
+      </c>
+      <c r="F6" s="44">
+        <v>0.206660698989033</v>
+      </c>
+      <c r="G6" s="44">
+        <v>256</v>
+      </c>
+      <c r="H6" s="44">
+        <v>0.189240486269389</v>
+      </c>
+      <c r="I6" s="44">
+        <v>128</v>
+      </c>
+      <c r="J6" s="47">
+        <v>1.0642869103081201</v>
+      </c>
+      <c r="K6" s="44">
+        <v>172</v>
+      </c>
+      <c r="L6" s="46">
+        <v>2.09442010603447</v>
+      </c>
+      <c r="M6" s="43">
+        <v>576</v>
+      </c>
+      <c r="N6" s="47">
+        <v>6.0084970312274402E-15</v>
+      </c>
+      <c r="O6" s="44">
+        <v>512</v>
+      </c>
+      <c r="P6" s="44">
+        <v>7.2707237794323301E-3</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>256</v>
+      </c>
+      <c r="R6" s="47">
+        <v>8.0742880682756202E-2</v>
+      </c>
+      <c r="S6" s="44">
+        <v>344</v>
+      </c>
+      <c r="T6" s="47">
+        <v>0.61230076410364398</v>
+      </c>
+      <c r="U6" s="44">
+        <v>256</v>
+      </c>
+      <c r="V6" s="46">
+        <v>0.113744768248721</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>65536</v>
+      </c>
+      <c r="B7" s="25">
+        <f t="shared" si="2"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="C7" s="25">
+        <f t="shared" si="0"/>
+        <v>6.103515625E-4</v>
+      </c>
+      <c r="D7" s="25">
+        <f t="shared" si="1"/>
+        <v>2.384185791015625E-6</v>
+      </c>
+      <c r="E7" s="43">
+        <v>1024</v>
+      </c>
+      <c r="F7" s="44">
+        <v>5.1812164029267901E-2</v>
+      </c>
+      <c r="G7" s="44">
+        <v>1024</v>
+      </c>
+      <c r="H7" s="44">
+        <v>4.7254594497097901E-2</v>
+      </c>
+      <c r="I7" s="44">
+        <v>440</v>
+      </c>
+      <c r="J7" s="47">
+        <v>1.4890730943887001</v>
+      </c>
+      <c r="K7" s="44">
+        <v>2212</v>
+      </c>
+      <c r="L7" s="46">
+        <v>0.47865451592365599</v>
+      </c>
+      <c r="M7" s="43">
+        <v>2304</v>
+      </c>
+      <c r="N7" s="47">
+        <v>1.2863932227470699E-14</v>
+      </c>
+      <c r="O7" s="44">
+        <v>2048</v>
+      </c>
+      <c r="P7" s="44">
+        <v>9.2094511558979701E-4</v>
+      </c>
+      <c r="Q7" s="44">
+        <v>880</v>
+      </c>
+      <c r="R7" s="47">
+        <v>1.44469986169836E-2</v>
+      </c>
+      <c r="S7" s="44">
+        <v>1072</v>
+      </c>
+      <c r="T7" s="47">
+        <v>1.3397457791017E-2</v>
+      </c>
+      <c r="U7" s="44">
+        <v>896</v>
+      </c>
+      <c r="V7" s="46">
+        <v>3.6155144182058001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>250000</v>
+      </c>
+      <c r="B8" s="25">
+        <f>1/250</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C8" s="25">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999999E-4</v>
+      </c>
+      <c r="D8" s="25">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-7</v>
+      </c>
+      <c r="E8" s="43">
+        <v>4096</v>
+      </c>
+      <c r="F8" s="44">
+        <v>1.2968167697866699E-2</v>
+      </c>
+      <c r="G8" s="44">
+        <v>4096</v>
+      </c>
+      <c r="H8" s="44">
+        <v>1.18098910153499E-2</v>
+      </c>
+      <c r="I8" s="44">
+        <v>1640</v>
+      </c>
+      <c r="J8" s="47">
+        <v>1.15780070020932</v>
+      </c>
+      <c r="K8" s="44">
+        <v>8644</v>
+      </c>
+      <c r="L8" s="46">
+        <v>9.5366481541707904E-2</v>
+      </c>
+      <c r="M8" s="43">
+        <v>9216</v>
+      </c>
+      <c r="N8" s="47">
+        <v>1.85454352663668E-14</v>
+      </c>
+      <c r="O8" s="44">
+        <v>8192</v>
+      </c>
+      <c r="P8" s="44">
+        <v>1.16770295444356E-4</v>
+      </c>
+      <c r="Q8" s="44">
+        <v>3280</v>
+      </c>
+      <c r="R8" s="47">
+        <v>1.9808011726754099E-3</v>
+      </c>
+      <c r="S8" s="44">
+        <v>4424</v>
+      </c>
+      <c r="T8" s="47">
+        <v>2.2061235561505002E-3</v>
+      </c>
+      <c r="U8" s="44">
+        <v>3272</v>
+      </c>
+      <c r="V8" s="46">
+        <v>1.09116262033231E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E9" s="43">
+        <v>16384</v>
+      </c>
+      <c r="F9" s="44">
+        <v>3.2436799318507899E-3</v>
+      </c>
+      <c r="G9" s="44">
+        <v>16384</v>
+      </c>
+      <c r="H9" s="44">
+        <v>2.9522298143167601E-3</v>
+      </c>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="43">
+        <v>36864</v>
+      </c>
+      <c r="N9" s="47">
+        <v>3.7159313054459903E-14</v>
+      </c>
+      <c r="O9" s="44">
+        <v>32768</v>
+      </c>
+      <c r="P9" s="47">
+        <v>1.51326488849241E-5</v>
+      </c>
+      <c r="Q9" s="44">
+        <v>12664</v>
+      </c>
+      <c r="R9" s="47">
+        <v>4.2034561665896399E-4</v>
+      </c>
+      <c r="S9" s="44">
+        <v>17288</v>
+      </c>
+      <c r="T9" s="47">
+        <v>5.9478686499189496E-3</v>
+      </c>
+      <c r="U9" s="44">
+        <v>12960</v>
+      </c>
+      <c r="V9" s="46">
+        <v>1.22127618865365E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E10" s="43">
+        <v>65536</v>
+      </c>
+      <c r="F10" s="44">
+        <v>8.1110695211347597E-4</v>
+      </c>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="43">
+        <v>147456</v>
+      </c>
+      <c r="N10" s="47">
+        <v>4.3167141395578798E-14</v>
+      </c>
+      <c r="O10" s="44">
+        <v>131072</v>
+      </c>
+      <c r="P10" s="47">
+        <v>2.1250912616835202E-6</v>
+      </c>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="45"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="45"/>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E12" s="43"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="44"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="45"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E13" s="43"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="45"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E15" s="43"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="45"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E16" s="43"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="45"/>
+    </row>
+    <row r="17" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E17" s="43"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="44"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="45"/>
+    </row>
+    <row r="18" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="45"/>
+    </row>
+    <row r="19" spans="5:22" x14ac:dyDescent="0.25">
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="44"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="45"/>
+    </row>
+    <row r="20" spans="5:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="48"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="M1:V1"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -8424,29 +10662,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="17"/>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="P1" s="26" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="P1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -8476,22 +10714,22 @@
       <c r="I2" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26" t="s">
+      <c r="L2" s="27"/>
+      <c r="M2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="P2" s="26" t="s">
+      <c r="N2" s="27"/>
+      <c r="P2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26" t="s">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="26"/>
+      <c r="S2" s="27"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
@@ -8892,7 +11130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -8906,48 +11144,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -9054,7 +11292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
@@ -9068,48 +11306,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="27" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -9481,7 +11719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -9495,40 +11733,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">

</xml_diff>

<commit_message>
still getting fourier working
</commit_message>
<xml_diff>
--- a/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
+++ b/Codes/MATLAB/POLYFEM/outputs/Transport_MMS/simple_scaling_MMS.xlsx
@@ -729,6 +729,15 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -738,27 +747,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,6 +754,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -783,6 +783,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -793,12 +799,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3569,11 +3569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="187826352"/>
-        <c:axId val="187826912"/>
+        <c:axId val="197967520"/>
+        <c:axId val="197968080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="187826352"/>
+        <c:axId val="197967520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3687,12 +3687,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187826912"/>
+        <c:crossAx val="197968080"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="187826912"/>
+        <c:axId val="197968080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3807,7 +3807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187826352"/>
+        <c:crossAx val="197967520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4277,11 +4277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189676016"/>
-        <c:axId val="189676576"/>
+        <c:axId val="199862960"/>
+        <c:axId val="199863520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189676016"/>
+        <c:axId val="199862960"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4339,12 +4339,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189676576"/>
+        <c:crossAx val="199863520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189676576"/>
+        <c:axId val="199863520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4402,7 +4402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189676016"/>
+        <c:crossAx val="199862960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4789,11 +4789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189680496"/>
-        <c:axId val="189681056"/>
+        <c:axId val="199867440"/>
+        <c:axId val="199868000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189680496"/>
+        <c:axId val="199867440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4851,12 +4851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189681056"/>
+        <c:crossAx val="199868000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189681056"/>
+        <c:axId val="199868000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4914,7 +4914,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189680496"/>
+        <c:crossAx val="199867440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5979,11 +5979,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188396080"/>
-        <c:axId val="188396640"/>
+        <c:axId val="197975920"/>
+        <c:axId val="197976480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188396080"/>
+        <c:axId val="197975920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6098,12 +6098,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188396640"/>
+        <c:crossAx val="197976480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188396640"/>
+        <c:axId val="197976480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6219,7 +6219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188396080"/>
+        <c:crossAx val="197975920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7285,11 +7285,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188404480"/>
-        <c:axId val="188405040"/>
+        <c:axId val="199162384"/>
+        <c:axId val="199162944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188404480"/>
+        <c:axId val="199162384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7404,12 +7404,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188405040"/>
+        <c:crossAx val="199162944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188405040"/>
+        <c:axId val="199162944"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7525,7 +7525,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188404480"/>
+        <c:crossAx val="199162384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8615,11 +8615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189161408"/>
-        <c:axId val="189161968"/>
+        <c:axId val="199170784"/>
+        <c:axId val="199171344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189161408"/>
+        <c:axId val="199170784"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8735,12 +8735,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189161968"/>
+        <c:crossAx val="199171344"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189161968"/>
+        <c:axId val="199171344"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8856,7 +8856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189161408"/>
+        <c:crossAx val="199170784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11766,11 +11766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189172048"/>
-        <c:axId val="189172608"/>
+        <c:axId val="199411040"/>
+        <c:axId val="199411600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189172048"/>
+        <c:axId val="199411040"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -11829,12 +11829,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189172608"/>
+        <c:crossAx val="199411600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189172608"/>
+        <c:axId val="199411600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -11894,7 +11894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189172048"/>
+        <c:crossAx val="199411040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13155,11 +13155,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188658608"/>
-        <c:axId val="188659168"/>
+        <c:axId val="199419440"/>
+        <c:axId val="198959280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188658608"/>
+        <c:axId val="199419440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -13219,12 +13219,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188659168"/>
+        <c:crossAx val="198959280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188659168"/>
+        <c:axId val="198959280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -13282,7 +13282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188658608"/>
+        <c:crossAx val="199419440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13934,11 +13934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188664768"/>
-        <c:axId val="188665328"/>
+        <c:axId val="198964880"/>
+        <c:axId val="198965440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188664768"/>
+        <c:axId val="198964880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14052,12 +14052,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188665328"/>
+        <c:crossAx val="198965440"/>
         <c:crossesAt val="10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188665328"/>
+        <c:axId val="198965440"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14170,7 +14170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188664768"/>
+        <c:crossAx val="198964880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14722,11 +14722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188670368"/>
-        <c:axId val="189665376"/>
+        <c:axId val="198970480"/>
+        <c:axId val="198971040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188670368"/>
+        <c:axId val="198970480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14784,12 +14784,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189665376"/>
+        <c:crossAx val="198971040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189665376"/>
+        <c:axId val="198971040"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -14847,7 +14847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188670368"/>
+        <c:crossAx val="198970480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15452,11 +15452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="189670976"/>
-        <c:axId val="189671536"/>
+        <c:axId val="199857920"/>
+        <c:axId val="199858480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="189670976"/>
+        <c:axId val="199857920"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -15514,12 +15514,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189671536"/>
+        <c:crossAx val="199858480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="189671536"/>
+        <c:axId val="199858480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -15577,7 +15577,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189670976"/>
+        <c:crossAx val="199857920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22438,16 +22438,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="68"/>
       <c r="I1" s="87" t="s">
         <v>17</v>
       </c>
@@ -22865,12 +22865,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="72"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="68"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="87" t="s">
@@ -23046,8 +23046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BW28" sqref="BW28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23079,50 +23079,50 @@
       <c r="D1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="68" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="69"/>
-      <c r="AP1" s="69"/>
-      <c r="AQ1" s="69"/>
-      <c r="AR1" s="69"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="61"/>
+      <c r="AF1" s="61"/>
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="61"/>
+      <c r="AO1" s="61"/>
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="61"/>
+      <c r="AR1" s="61"/>
       <c r="AS1" t="s">
         <v>34</v>
       </c>
@@ -23156,90 +23156,90 @@
         <f>A2^(-2)*100</f>
         <v>100</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60" t="s">
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="71" t="s">
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
+      <c r="AD2" s="63"/>
+      <c r="AE2" s="63"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="72"/>
-      <c r="AS2" s="68" t="s">
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="65"/>
+      <c r="AM2" s="65"/>
+      <c r="AN2" s="65"/>
+      <c r="AO2" s="65"/>
+      <c r="AP2" s="65"/>
+      <c r="AQ2" s="65"/>
+      <c r="AR2" s="68"/>
+      <c r="AS2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="AT2" s="69"/>
-      <c r="AU2" s="69"/>
-      <c r="AV2" s="69"/>
-      <c r="AW2" s="69"/>
-      <c r="AX2" s="69"/>
-      <c r="AY2" s="69"/>
-      <c r="AZ2" s="69"/>
-      <c r="BA2" s="69"/>
-      <c r="BB2" s="69"/>
-      <c r="BC2" s="69"/>
-      <c r="BD2" s="69"/>
-      <c r="BE2" s="69"/>
-      <c r="BF2" s="69"/>
-      <c r="BG2" s="69"/>
-      <c r="BH2" s="69"/>
-      <c r="BI2" s="69"/>
-      <c r="BJ2" s="69"/>
-      <c r="BK2" s="69"/>
-      <c r="BL2" s="69"/>
-      <c r="BM2" s="69"/>
-      <c r="BN2" s="69"/>
-      <c r="BO2" s="69"/>
-      <c r="BP2" s="69"/>
-      <c r="BQ2" s="67" t="s">
+      <c r="AT2" s="61"/>
+      <c r="AU2" s="61"/>
+      <c r="AV2" s="61"/>
+      <c r="AW2" s="61"/>
+      <c r="AX2" s="61"/>
+      <c r="AY2" s="61"/>
+      <c r="AZ2" s="61"/>
+      <c r="BA2" s="61"/>
+      <c r="BB2" s="61"/>
+      <c r="BC2" s="61"/>
+      <c r="BD2" s="61"/>
+      <c r="BE2" s="61"/>
+      <c r="BF2" s="61"/>
+      <c r="BG2" s="61"/>
+      <c r="BH2" s="61"/>
+      <c r="BI2" s="61"/>
+      <c r="BJ2" s="61"/>
+      <c r="BK2" s="61"/>
+      <c r="BL2" s="61"/>
+      <c r="BM2" s="61"/>
+      <c r="BN2" s="61"/>
+      <c r="BO2" s="61"/>
+      <c r="BP2" s="61"/>
+      <c r="BQ2" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="BR2" s="67"/>
-      <c r="BS2" s="67"/>
-      <c r="BT2" s="67"/>
-      <c r="BU2" s="67"/>
-      <c r="BV2" s="67"/>
-      <c r="BW2" s="67"/>
-      <c r="BX2" s="67"/>
+      <c r="BR2" s="70"/>
+      <c r="BS2" s="70"/>
+      <c r="BT2" s="70"/>
+      <c r="BU2" s="70"/>
+      <c r="BV2" s="70"/>
+      <c r="BW2" s="70"/>
+      <c r="BX2" s="70"/>
     </row>
     <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -23257,94 +23257,94 @@
         <f t="shared" ref="D3:D9" si="2">A3^(-2)*100</f>
         <v>1</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60" t="s">
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60" t="s">
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
+      <c r="V3" s="63"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="60"/>
-      <c r="AA3" s="60"/>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="60"/>
-      <c r="AF3" s="60"/>
-      <c r="AG3" s="60"/>
-      <c r="AH3" s="60"/>
-      <c r="AI3" s="63" t="s">
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="63"/>
+      <c r="AF3" s="63"/>
+      <c r="AG3" s="63"/>
+      <c r="AH3" s="63"/>
+      <c r="AI3" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65" t="s">
+      <c r="AJ3" s="72"/>
+      <c r="AK3" s="72"/>
+      <c r="AL3" s="72"/>
+      <c r="AM3" s="72"/>
+      <c r="AN3" s="72"/>
+      <c r="AO3" s="72"/>
+      <c r="AP3" s="72"/>
+      <c r="AQ3" s="72"/>
+      <c r="AR3" s="69"/>
+      <c r="AS3" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="AT3" s="60"/>
-      <c r="AU3" s="60"/>
-      <c r="AV3" s="60"/>
-      <c r="AW3" s="60"/>
-      <c r="AX3" s="60"/>
-      <c r="AY3" s="60"/>
-      <c r="AZ3" s="60"/>
-      <c r="BA3" s="60" t="s">
+      <c r="AT3" s="63"/>
+      <c r="AU3" s="63"/>
+      <c r="AV3" s="63"/>
+      <c r="AW3" s="63"/>
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="63"/>
+      <c r="AZ3" s="63"/>
+      <c r="BA3" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="BB3" s="60"/>
-      <c r="BC3" s="60"/>
-      <c r="BD3" s="60"/>
-      <c r="BE3" s="60"/>
-      <c r="BF3" s="60"/>
-      <c r="BG3" s="60"/>
-      <c r="BH3" s="60"/>
-      <c r="BI3" s="60" t="s">
+      <c r="BB3" s="63"/>
+      <c r="BC3" s="63"/>
+      <c r="BD3" s="63"/>
+      <c r="BE3" s="63"/>
+      <c r="BF3" s="63"/>
+      <c r="BG3" s="63"/>
+      <c r="BH3" s="63"/>
+      <c r="BI3" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="BJ3" s="60"/>
-      <c r="BK3" s="60"/>
-      <c r="BL3" s="60"/>
-      <c r="BM3" s="60"/>
-      <c r="BN3" s="60"/>
-      <c r="BO3" s="60"/>
-      <c r="BP3" s="60"/>
-      <c r="BQ3" s="70" t="s">
+      <c r="BJ3" s="63"/>
+      <c r="BK3" s="63"/>
+      <c r="BL3" s="63"/>
+      <c r="BM3" s="63"/>
+      <c r="BN3" s="63"/>
+      <c r="BO3" s="63"/>
+      <c r="BP3" s="63"/>
+      <c r="BQ3" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="BR3" s="70"/>
-      <c r="BS3" s="70"/>
-      <c r="BT3" s="70"/>
-      <c r="BU3" s="70"/>
-      <c r="BV3" s="70"/>
-      <c r="BW3" s="70"/>
-      <c r="BX3" s="70"/>
+      <c r="BR3" s="66"/>
+      <c r="BS3" s="66"/>
+      <c r="BT3" s="66"/>
+      <c r="BU3" s="66"/>
+      <c r="BV3" s="66"/>
+      <c r="BW3" s="66"/>
+      <c r="BX3" s="66"/>
     </row>
     <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -23362,150 +23362,150 @@
         <f t="shared" si="2"/>
         <v>0.01</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61" t="s">
+      <c r="F4" s="64"/>
+      <c r="G4" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61" t="s">
+      <c r="H4" s="64"/>
+      <c r="I4" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61" t="s">
+      <c r="J4" s="64"/>
+      <c r="K4" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61" t="s">
+      <c r="L4" s="64"/>
+      <c r="M4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61" t="s">
+      <c r="N4" s="64"/>
+      <c r="O4" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="62" t="s">
+      <c r="P4" s="64"/>
+      <c r="Q4" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62" t="s">
+      <c r="R4" s="65"/>
+      <c r="S4" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62" t="s">
+      <c r="T4" s="65"/>
+      <c r="U4" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="V4" s="62"/>
-      <c r="W4" s="61" t="s">
+      <c r="V4" s="65"/>
+      <c r="W4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61" t="s">
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61" t="s">
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61" t="s">
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="61" t="s">
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="AF4" s="61"/>
-      <c r="AG4" s="61" t="s">
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="61" t="s">
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="AJ4" s="61"/>
-      <c r="AK4" s="62" t="s">
+      <c r="AJ4" s="64"/>
+      <c r="AK4" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="AL4" s="62"/>
-      <c r="AM4" s="62" t="s">
+      <c r="AL4" s="65"/>
+      <c r="AM4" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="AN4" s="62"/>
-      <c r="AO4" s="62" t="s">
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="AP4" s="62"/>
-      <c r="AQ4" s="61" t="s">
+      <c r="AP4" s="65"/>
+      <c r="AQ4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AR4" s="61"/>
-      <c r="AS4" s="66" t="s">
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66" t="s">
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="66" t="s">
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="AX4" s="66"/>
-      <c r="AY4" s="66" t="s">
+      <c r="AX4" s="62"/>
+      <c r="AY4" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="AZ4" s="66"/>
-      <c r="BA4" s="66" t="s">
+      <c r="AZ4" s="62"/>
+      <c r="BA4" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="BB4" s="66"/>
-      <c r="BC4" s="66" t="s">
+      <c r="BB4" s="62"/>
+      <c r="BC4" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="BD4" s="66"/>
-      <c r="BE4" s="66" t="s">
+      <c r="BD4" s="62"/>
+      <c r="BE4" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="BF4" s="66"/>
-      <c r="BG4" s="66" t="s">
+      <c r="BF4" s="62"/>
+      <c r="BG4" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="BH4" s="66"/>
-      <c r="BI4" s="66" t="s">
+      <c r="BH4" s="62"/>
+      <c r="BI4" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="BJ4" s="66"/>
-      <c r="BK4" s="66" t="s">
+      <c r="BJ4" s="62"/>
+      <c r="BK4" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="BL4" s="66"/>
-      <c r="BM4" s="66" t="s">
+      <c r="BL4" s="62"/>
+      <c r="BM4" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="BN4" s="66"/>
-      <c r="BO4" s="66" t="s">
+      <c r="BN4" s="62"/>
+      <c r="BO4" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="BP4" s="66"/>
-      <c r="BQ4" s="66" t="s">
+      <c r="BP4" s="62"/>
+      <c r="BQ4" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="BR4" s="66"/>
-      <c r="BS4" s="66" t="s">
+      <c r="BR4" s="62"/>
+      <c r="BS4" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="BT4" s="66"/>
-      <c r="BU4" s="66" t="s">
+      <c r="BT4" s="62"/>
+      <c r="BU4" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="BV4" s="66"/>
-      <c r="BW4" s="66" t="s">
+      <c r="BV4" s="62"/>
+      <c r="BW4" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="BX4" s="66"/>
+      <c r="BX4" s="62"/>
     </row>
     <row r="5" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -25776,6 +25776,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="Y2:AH2"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AI3:AR3"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="Y3:AH3"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="E1:X1"/>
+    <mergeCell ref="BQ4:BR4"/>
+    <mergeCell ref="BA3:BH3"/>
+    <mergeCell ref="BA4:BB4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AS3:AZ3"/>
+    <mergeCell ref="O3:X3"/>
+    <mergeCell ref="O2:X2"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="BQ2:BX2"/>
     <mergeCell ref="Y1:AR1"/>
     <mergeCell ref="BS4:BT4"/>
     <mergeCell ref="BW4:BX4"/>
@@ -25792,42 +25828,6 @@
     <mergeCell ref="AM4:AN4"/>
     <mergeCell ref="AK4:AL4"/>
     <mergeCell ref="AI2:AR2"/>
-    <mergeCell ref="E1:X1"/>
-    <mergeCell ref="BQ4:BR4"/>
-    <mergeCell ref="BA3:BH3"/>
-    <mergeCell ref="BA4:BB4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AS3:AZ3"/>
-    <mergeCell ref="O3:X3"/>
-    <mergeCell ref="O2:X2"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="BQ2:BX2"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AI3:AR3"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="Y3:AH3"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="Y2:AH2"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30132,11 +30132,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="Q1:R1"/>
@@ -30144,6 +30139,11 @@
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -30170,33 +30170,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61" t="s">
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61" t="s">
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -30985,41 +30985,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="L1" s="61" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="L1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61" t="s">
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="61"/>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="61"/>
-      <c r="AE1" s="61"/>
-      <c r="AF1" s="61"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -31061,38 +31061,38 @@
       <c r="P2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="61" t="s">
+      <c r="Q2" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61" t="s">
+      <c r="R2" s="64"/>
+      <c r="S2" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61" t="s">
+      <c r="T2" s="64"/>
+      <c r="U2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61" t="s">
+      <c r="V2" s="64"/>
+      <c r="W2" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61" t="s">
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61" t="s">
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61" t="s">
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61" t="s">
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="61"/>
+      <c r="AF2" s="64"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -31997,28 +31997,28 @@
       <c r="D1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="78" t="s">
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="80"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
+      <c r="S1" s="81"/>
+      <c r="T1" s="81"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="82"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
@@ -32036,32 +32036,32 @@
         <f>B2^3*5</f>
         <v>7.8125E-2</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82" t="s">
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="81" t="s">
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82" t="s">
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="83"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="79"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
@@ -32079,42 +32079,42 @@
         <f t="shared" ref="D3:D8" si="1">B3^3*5</f>
         <v>9.765625E-3</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82" t="s">
+      <c r="F3" s="78"/>
+      <c r="G3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82" t="s">
+      <c r="H3" s="78"/>
+      <c r="I3" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82" t="s">
+      <c r="J3" s="78"/>
+      <c r="K3" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="83"/>
-      <c r="M3" s="81" t="s">
+      <c r="L3" s="79"/>
+      <c r="M3" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82" t="s">
+      <c r="N3" s="78"/>
+      <c r="O3" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82" t="s">
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82" t="s">
+      <c r="R3" s="78"/>
+      <c r="S3" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82" t="s">
+      <c r="T3" s="78"/>
+      <c r="U3" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="83"/>
+      <c r="V3" s="79"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
@@ -32753,11 +32753,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="M1:V1"/>
-    <mergeCell ref="M3:N3"/>
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
@@ -32769,6 +32764,11 @@
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="M1:V1"/>
+    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32790,29 +32790,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
       <c r="I1" s="16"/>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="P1" s="67" t="s">
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="P1" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
@@ -32842,22 +32842,22 @@
       <c r="I2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67" t="s">
+      <c r="L2" s="70"/>
+      <c r="M2" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="P2" s="67" t="s">
+      <c r="N2" s="70"/>
+      <c r="P2" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67" t="s">
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="67"/>
+      <c r="S2" s="70"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
@@ -33272,16 +33272,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="68"/>
       <c r="I1" s="87" t="s">
         <v>17</v>
       </c>

</xml_diff>